<commit_message>
evidencias fotograficas y marco teorico completo
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unaledu-my.sharepoint.com/personal/scarvajal_unal_edu_co/Documents/MNL/Tarea 1 Hielos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/80f5a00308bb530a/Documents/GitHub/Tarea_Hielos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="8_{749A67EE-F898-43C0-ABD5-FD20B3382A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36E79F70-ED42-4AF9-B3C1-E85914DDFF7C}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="8_{749A67EE-F898-43C0-ABD5-FD20B3382A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3F088F5-EE92-4F4C-B684-2FF23E586B00}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{EA4199BD-6337-4503-B5D5-74364C08036D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{EA4199BD-6337-4503-B5D5-74364C08036D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -88,24 +88,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person0.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person1.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person2.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -403,11 +387,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE038D40-D6B3-4C74-BFBE-F896323A6DAF}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C5" sqref="A2:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -820,9 +804,9 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C36">
-    <sortCondition ref="A2:A36"/>
-    <sortCondition ref="B2:B36"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C37">
+    <sortCondition ref="A2:A37"/>
+    <sortCondition ref="B2:B37"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>